<commit_message>
first published version... added detail data, business report, etc.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.king\OneDrive - UiPath\Documents\Diamondback\OpenTicket_Audit\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/richard_king_uipath_com/Documents/Documents/Diamondback/OpenTicket_Audit/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948640E4-A16E-4BDC-ADC1-8EFB9DBC289F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{948640E4-A16E-4BDC-ADC1-8EFB9DBC289F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71A774DA-24B4-41C5-B567-6A42476BD7BA}"/>
   <bookViews>
-    <workbookView xWindow="-29100" yWindow="-7590" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>FolderPathForResultsFiles</t>
+  </si>
+  <si>
+    <t>RequisitionerFail</t>
+  </si>
+  <si>
+    <t>RequisitionerPass</t>
   </si>
 </sst>
 </file>
@@ -2734,7 +2740,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2829,8 +2835,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added assets to config.   On technical report, added Correct answer.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/richard_king_uipath_com/Documents/Documents/Diamondback/OpenTicket_Audit/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{948640E4-A16E-4BDC-ADC1-8EFB9DBC289F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71A774DA-24B4-41C5-B567-6A42476BD7BA}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{948640E4-A16E-4BDC-ADC1-8EFB9DBC289F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A42D7E-003D-4EBA-8CDD-A642C01223A5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29100" yWindow="-7590" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>RequisitionerPass</t>
+  </si>
+  <si>
+    <t>Price Book Alert yellow and red</t>
+  </si>
+  <si>
+    <t>If the text from the screen is found using a .contains function.</t>
+  </si>
+  <si>
+    <t>100% of line items not covered by the price book; 50% of line items not covered by the price book</t>
   </si>
 </sst>
 </file>
@@ -160,6 +169,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -244,6 +254,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1616,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1667,7 +1681,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>28</v>
@@ -1752,7 +1766,17 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2739,7 +2763,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implemented ticket test list feature.  extracted run agent to new workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/richard_king_uipath_com/Documents/Documents/Diamondback/OpenTicket_Audit/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{948640E4-A16E-4BDC-ADC1-8EFB9DBC289F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A42D7E-003D-4EBA-8CDD-A642C01223A5}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{948640E4-A16E-4BDC-ADC1-8EFB9DBC289F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DDD297E-AE6B-40F3-9918-01CAD35DFF25}"/>
   <bookViews>
-    <workbookView xWindow="-29100" yWindow="-7590" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29100" yWindow="-7590" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>100% of line items not covered by the price book; 50% of line items not covered by the price book</t>
+  </si>
+  <si>
+    <t>TestTicketsList</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2763,8 +2766,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2875,7 +2878,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added report filenames to config and assets.  Added timestamp to report files.  Fixed problem with logon screen.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/richard_king_uipath_com/Documents/Documents/Diamondback/OpenTicket_Audit/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{948640E4-A16E-4BDC-ADC1-8EFB9DBC289F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DDD297E-AE6B-40F3-9918-01CAD35DFF25}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{948640E4-A16E-4BDC-ADC1-8EFB9DBC289F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C81FE3B-E038-4422-A86A-0B0A1F924972}"/>
   <bookViews>
-    <workbookView xWindow="-29100" yWindow="-7590" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21795" yWindow="-4965" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -155,13 +155,19 @@
   </si>
   <si>
     <t>TestTicketsList</t>
+  </si>
+  <si>
+    <t>TechnicalResultsFileName</t>
+  </si>
+  <si>
+    <t>BusinessResultsFileName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,6 +210,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -225,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -242,6 +254,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2767,7 +2780,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2886,8 +2899,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>